<commit_message>
minor fixes in spreadsheet
</commit_message>
<xml_diff>
--- a/evaluation/dstc7-task2-automatic_scores.xlsx
+++ b/evaluation/dstc7-task2-automatic_scores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mgalley\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proj\dstc7\reddit\main\official\DSTC7-End-to-End-Conversation-Modeling\evaluation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B93EF18-3F8B-4AE4-8B02-967DC98DDA78}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{391D5573-5356-4061-AFCC-E791296027A7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="13665" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,15 +1518,6 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1542,20 +1533,29 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="55" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -2430,9 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D31"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2513,7 +2511,7 @@
       <c r="B2" s="82">
         <v>2208</v>
       </c>
-      <c r="C2" s="129" t="s">
+      <c r="C2" s="126" t="s">
         <v>67</v>
       </c>
       <c r="D2" s="121" t="s">
@@ -2575,7 +2573,7 @@
       <c r="B3" s="82">
         <v>2208</v>
       </c>
-      <c r="C3" s="130" t="s">
+      <c r="C3" s="127" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="122" t="s">
@@ -2637,7 +2635,7 @@
       <c r="B4" s="82">
         <v>2208</v>
       </c>
-      <c r="C4" s="130"/>
+      <c r="C4" s="127"/>
       <c r="D4" s="122"/>
       <c r="E4" s="2">
         <v>0.84889999999999999</v>
@@ -2695,7 +2693,7 @@
       <c r="B5" s="83">
         <v>2208</v>
       </c>
-      <c r="C5" s="130" t="s">
+      <c r="C5" s="127" t="s">
         <v>67</v>
       </c>
       <c r="D5" s="122" t="s">
@@ -2757,7 +2755,7 @@
       <c r="B6" s="84">
         <v>2208</v>
       </c>
-      <c r="C6" s="131" t="s">
+      <c r="C6" s="128" t="s">
         <v>67</v>
       </c>
       <c r="D6" s="123" t="s">
@@ -2819,7 +2817,7 @@
       <c r="B7" s="85">
         <v>2208</v>
       </c>
-      <c r="C7" s="132" t="s">
+      <c r="C7" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D7" s="124" t="s">
@@ -2881,7 +2879,7 @@
       <c r="B8" s="86">
         <v>2208</v>
       </c>
-      <c r="C8" s="133" t="s">
+      <c r="C8" s="130" t="s">
         <v>30</v>
       </c>
       <c r="D8" s="125" t="s">
@@ -2943,7 +2941,7 @@
       <c r="B9" s="87">
         <v>2208</v>
       </c>
-      <c r="C9" s="131" t="s">
+      <c r="C9" s="128" t="s">
         <v>67</v>
       </c>
       <c r="D9" s="123" t="s">
@@ -3005,7 +3003,7 @@
       <c r="B10" s="86">
         <v>2208</v>
       </c>
-      <c r="C10" s="133" t="s">
+      <c r="C10" s="130" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="125" t="s">
@@ -3067,7 +3065,7 @@
       <c r="B11" s="84">
         <v>2208</v>
       </c>
-      <c r="C11" s="131" t="s">
+      <c r="C11" s="128" t="s">
         <v>67</v>
       </c>
       <c r="D11" s="123" t="s">
@@ -3129,7 +3127,7 @@
       <c r="B12" s="85">
         <v>2208</v>
       </c>
-      <c r="C12" s="132" t="s">
+      <c r="C12" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D12" s="124" t="s">
@@ -3191,7 +3189,7 @@
       <c r="B13" s="85">
         <v>2208</v>
       </c>
-      <c r="C13" s="132" t="s">
+      <c r="C13" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D13" s="124" t="s">
@@ -3253,7 +3251,7 @@
       <c r="B14" s="85">
         <v>2208</v>
       </c>
-      <c r="C14" s="132" t="s">
+      <c r="C14" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D14" s="124" t="s">
@@ -3315,7 +3313,7 @@
       <c r="B15" s="86">
         <v>2208</v>
       </c>
-      <c r="C15" s="133" t="s">
+      <c r="C15" s="130" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="125" t="s">
@@ -3377,7 +3375,7 @@
       <c r="B16" s="84">
         <v>2208</v>
       </c>
-      <c r="C16" s="131" t="s">
+      <c r="C16" s="128" t="s">
         <v>67</v>
       </c>
       <c r="D16" s="123" t="s">
@@ -3439,7 +3437,7 @@
       <c r="B17" s="85">
         <v>2208</v>
       </c>
-      <c r="C17" s="132" t="s">
+      <c r="C17" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="124" t="s">
@@ -3501,7 +3499,7 @@
       <c r="B18" s="85">
         <v>2208</v>
       </c>
-      <c r="C18" s="132" t="s">
+      <c r="C18" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D18" s="124" t="s">
@@ -3563,7 +3561,7 @@
       <c r="B19" s="85">
         <v>2208</v>
       </c>
-      <c r="C19" s="132" t="s">
+      <c r="C19" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D19" s="124" t="s">
@@ -3625,7 +3623,7 @@
       <c r="B20" s="85">
         <v>2208</v>
       </c>
-      <c r="C20" s="132" t="s">
+      <c r="C20" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D20" s="124" t="s">
@@ -3687,7 +3685,7 @@
       <c r="B21" s="85">
         <v>2208</v>
       </c>
-      <c r="C21" s="132" t="s">
+      <c r="C21" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D21" s="124" t="s">
@@ -3749,7 +3747,7 @@
       <c r="B22" s="86">
         <v>2208</v>
       </c>
-      <c r="C22" s="133" t="s">
+      <c r="C22" s="130" t="s">
         <v>30</v>
       </c>
       <c r="D22" s="125" t="s">
@@ -3811,7 +3809,7 @@
       <c r="B23" s="84">
         <v>2208</v>
       </c>
-      <c r="C23" s="131" t="s">
+      <c r="C23" s="128" t="s">
         <v>67</v>
       </c>
       <c r="D23" s="123" t="s">
@@ -3873,7 +3871,7 @@
       <c r="B24" s="85">
         <v>2208</v>
       </c>
-      <c r="C24" s="132" t="s">
+      <c r="C24" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D24" s="124" t="s">
@@ -3935,7 +3933,7 @@
       <c r="B25" s="85">
         <v>2208</v>
       </c>
-      <c r="C25" s="132" t="s">
+      <c r="C25" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="124" t="s">
@@ -3997,7 +3995,7 @@
       <c r="B26" s="86">
         <v>2208</v>
       </c>
-      <c r="C26" s="133" t="s">
+      <c r="C26" s="130" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="125" t="s">
@@ -4059,7 +4057,7 @@
       <c r="B27" s="84">
         <v>2208</v>
       </c>
-      <c r="C27" s="131" t="s">
+      <c r="C27" s="128" t="s">
         <v>67</v>
       </c>
       <c r="D27" s="123" t="s">
@@ -4121,7 +4119,7 @@
       <c r="B28" s="85">
         <v>2208</v>
       </c>
-      <c r="C28" s="132" t="s">
+      <c r="C28" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D28" s="124" t="s">
@@ -4183,7 +4181,7 @@
       <c r="B29" s="86">
         <v>2208</v>
       </c>
-      <c r="C29" s="133" t="s">
+      <c r="C29" s="130" t="s">
         <v>30</v>
       </c>
       <c r="D29" s="125" t="s">
@@ -4245,7 +4243,7 @@
       <c r="B30" s="85">
         <v>2208</v>
       </c>
-      <c r="C30" s="132" t="s">
+      <c r="C30" s="129" t="s">
         <v>67</v>
       </c>
       <c r="D30" s="124" t="s">
@@ -4307,7 +4305,7 @@
       <c r="B31" s="85">
         <v>2208</v>
       </c>
-      <c r="C31" s="132" t="s">
+      <c r="C31" s="129" t="s">
         <v>30</v>
       </c>
       <c r="D31" s="124" t="s">
@@ -4369,10 +4367,10 @@
       <c r="B32" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="134" t="s">
+      <c r="C32" s="133" t="s">
         <v>67</v>
       </c>
-      <c r="D32" s="126" t="s">
+      <c r="D32" s="134" t="s">
         <v>67</v>
       </c>
       <c r="E32" s="5">
@@ -4449,7 +4447,7 @@
       <c r="C33" s="135" t="s">
         <v>67</v>
       </c>
-      <c r="D33" s="127" t="s">
+      <c r="D33" s="136" t="s">
         <v>67</v>
       </c>
       <c r="E33" s="10">
@@ -4523,10 +4521,10 @@
       <c r="B34" s="110" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="136" t="s">
+      <c r="C34" s="137" t="s">
         <v>67</v>
       </c>
-      <c r="D34" s="128" t="s">
+      <c r="D34" s="138" t="s">
         <v>67</v>
       </c>
       <c r="E34" s="56">
@@ -4594,24 +4592,24 @@
       </c>
     </row>
     <row r="40" spans="1:20" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="138" t="s">
+      <c r="A40" s="132" t="s">
         <v>66</v>
       </c>
-      <c r="B40" s="138"/>
-      <c r="C40" s="138"/>
-      <c r="D40" s="138"/>
-      <c r="E40" s="138"/>
-      <c r="F40" s="138"/>
-      <c r="G40" s="138"/>
-      <c r="H40" s="138"/>
-      <c r="I40" s="138"/>
-      <c r="J40" s="138"/>
-      <c r="K40" s="138"/>
-      <c r="L40" s="138"/>
-      <c r="M40" s="138"/>
-      <c r="N40" s="138"/>
-      <c r="O40" s="138"/>
-      <c r="P40" s="138"/>
+      <c r="B40" s="132"/>
+      <c r="C40" s="132"/>
+      <c r="D40" s="132"/>
+      <c r="E40" s="132"/>
+      <c r="F40" s="132"/>
+      <c r="G40" s="132"/>
+      <c r="H40" s="132"/>
+      <c r="I40" s="132"/>
+      <c r="J40" s="132"/>
+      <c r="K40" s="132"/>
+      <c r="L40" s="132"/>
+      <c r="M40" s="132"/>
+      <c r="N40" s="132"/>
+      <c r="O40" s="132"/>
+      <c r="P40" s="132"/>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
@@ -4659,24 +4657,24 @@
       </c>
     </row>
     <row r="51" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="137" t="s">
+      <c r="A51" s="131" t="s">
         <v>63</v>
       </c>
-      <c r="B51" s="137"/>
-      <c r="C51" s="137"/>
-      <c r="D51" s="137"/>
-      <c r="E51" s="137"/>
-      <c r="F51" s="137"/>
-      <c r="G51" s="137"/>
-      <c r="H51" s="137"/>
-      <c r="I51" s="137"/>
-      <c r="J51" s="137"/>
-      <c r="K51" s="137"/>
-      <c r="L51" s="137"/>
-      <c r="M51" s="137"/>
-      <c r="N51" s="137"/>
-      <c r="O51" s="137"/>
-      <c r="P51" s="137"/>
+      <c r="B51" s="131"/>
+      <c r="C51" s="131"/>
+      <c r="D51" s="131"/>
+      <c r="E51" s="131"/>
+      <c r="F51" s="131"/>
+      <c r="G51" s="131"/>
+      <c r="H51" s="131"/>
+      <c r="I51" s="131"/>
+      <c r="J51" s="131"/>
+      <c r="K51" s="131"/>
+      <c r="L51" s="131"/>
+      <c r="M51" s="131"/>
+      <c r="N51" s="131"/>
+      <c r="O51" s="131"/>
+      <c r="P51" s="131"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">

</xml_diff>